<commit_message>
- nav bar container removed - excel triggers update
</commit_message>
<xml_diff>
--- a/src/ngDomo.xlsx
+++ b/src/ngDomo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Triggers" sheetId="1" r:id="rId1"/>
     <sheet name="Action" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="230">
   <si>
     <t>Comment</t>
   </si>
@@ -643,18 +643,9 @@
     <t>efd541</t>
   </si>
   <si>
-    <t>sonOff01.on</t>
-  </si>
-  <si>
-    <t>sonOff01.off</t>
-  </si>
-  <si>
     <t>Sony</t>
   </si>
   <si>
-    <t>Action A</t>
-  </si>
-  <si>
     <t>Action C</t>
   </si>
   <si>
@@ -707,12 +698,24 @@
   </si>
   <si>
     <t>f11</t>
+  </si>
+  <si>
+    <t>Action B</t>
+  </si>
+  <si>
+    <t>vpstudio.on</t>
+  </si>
+  <si>
+    <t>vpstudio.off</t>
+  </si>
+  <si>
+    <t>preamp.mute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1046,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1054,26 +1057,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1102,12 +1105,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>{'comment':'rxir sony 1-&gt;salon.1.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=11 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.1.on'}},</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F39" si="1">IF(B4&lt;&gt;"",B4&amp;"-&gt;"&amp;E4,"")</f>
+        <f t="shared" ref="F4:F45" si="1">IF(B4&lt;&gt;"",B4&amp;"-&gt;"&amp;E4,"")</f>
         <v>rxir sony 2-&gt;salon.2.on</v>
       </c>
       <c r="G4" t="str">
@@ -1161,23 +1164,23 @@
         <v>rxIR proto=4 code=811 (12 bits)</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H28" si="2">IF(OR(C4&lt;&gt;"", D4&lt;&gt;""),"home/domo/espIR01/event","")</f>
+        <f t="shared" ref="H4:H34" si="2">IF(OR(C4&lt;&gt;"", D4&lt;&gt;""),"home/domo/espIR01/event","")</f>
         <v>home/domo/espIR01/event</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I28" si="3">G4</f>
+        <f t="shared" ref="I4:I34" si="3">G4</f>
         <v>rxIR proto=4 code=811 (12 bits)</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J28" si="4">IF(E4&lt;&gt;"",E4,"")</f>
+        <f t="shared" ref="J4:J34" si="4">IF(E4&lt;&gt;"",E4,"")</f>
         <v>salon.2.on</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K28" si="5">IF(E4&lt;&gt;"","{'comment':'"&amp;F4&amp;"', 'type':'trgMqtt'," &amp;" 'topic':'"&amp;H4&amp;"', 'payload':'"&amp;I4&amp;"', 'command':{'type':'cmdCommand', 'id':'"&amp;J4&amp;"'}},","")</f>
+        <f t="shared" ref="K4:K34" si="5">IF(E4&lt;&gt;"","{'comment':'"&amp;F4&amp;"', 'type':'trgMqtt'," &amp;" 'topic':'"&amp;H4&amp;"', 'payload':'"&amp;I4&amp;"', 'command':{'type':'cmdCommand', 'id':'"&amp;J4&amp;"'}},","")</f>
         <v>{'comment':'rxir sony 2-&gt;salon.2.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=811 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.2.on'}},</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>{'comment':'rxir sony 3-&gt;salon.3.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=411 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.3.on'}},</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>{'comment':'rxir sony 4-&gt;salon.1.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=c11 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.1.off'}},</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>{'comment':'rxir sony 5-&gt;salon.2.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=211 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.2.off'}},</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>{'comment':'rxir sony 6-&gt;salon.3.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=a11 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.3.off'}},</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>{'comment':'rxir sony 7-&gt;salon.4.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=611 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.4.on'}},</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1387,12 +1390,12 @@
         <v>{'comment':'rxir sony 8-&gt;salon.5.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=e11 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.5.on'}},</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1422,9 +1425,9 @@
         <v>{'comment':'rxir sony &gt;10-&gt;salon.4.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=e51 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.4.off'}},</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C12" s="3">
         <v>51</v>
@@ -1457,7 +1460,7 @@
         <v>{'comment':'rxir sony 10-&gt;salon.5.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=51 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.5.off'}},</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -1492,12 +1495,12 @@
         <v>{'comment':'rxir sony 9-&gt;salon.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=111 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.on'}},</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E14" t="s">
         <v>51</v>
@@ -1527,12 +1530,12 @@
         <v>{'comment':'rxir sony clear-&gt;salon.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=f11 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.off'}},</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="3">
-        <v>111</v>
+        <v>491</v>
       </c>
       <c r="E15" t="s">
         <v>44</v>
@@ -1543,7 +1546,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>rxIR proto=4 code=111 (12 bits)</v>
+        <v>rxIR proto=4 code=491 (12 bits)</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
@@ -1551,7 +1554,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v>rxIR proto=4 code=111 (12 bits)</v>
+        <v>rxIR proto=4 code=491 (12 bits)</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="4"/>
@@ -1559,10 +1562,10 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="5"/>
-        <v>{'comment':'rxir sony plus-&gt;ampli.volp', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=111 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.volp'}},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+        <v>{'comment':'rxir sony plus-&gt;ampli.volp', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=491 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.volp'}},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>{'comment':'rxir sony minus-&gt;ampli.volm', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=c91 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.volm'}},</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>37</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>{'comment':'rxir sony play-&gt;tvon', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=4d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'tvon'}},</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -1667,7 +1670,7 @@
         <v>{'comment':'rxir sony pause-&gt;tvoff', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=9d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'tvoff'}},</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>{'comment':'rxir sony stop-&gt;ampli.mute', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=1d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.mute'}},</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>40</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>{'comment':'rxir sony prev-&gt;ampli.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.off'}},</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>41</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>{'comment':'rxir sony next-&gt;ampli.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=8d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'ampli.on'}},</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>42</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>{'comment':'rxir sony fbw-&gt;salon.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=cd1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.off'}},</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -1842,9 +1845,9 @@
         <v>{'comment':'rxir sony ffw-&gt;salon.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxIR proto=4 code=2d1 (12 bits)', 'command':{'type':'cmdCommand', 'id':'salon.on'}},</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1871,413 +1874,248 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="1"/>
-        <v>rxrf rf.b4.on-&gt;tvon</v>
-      </c>
-      <c r="G25" t="str">
-        <f>IF(C25&lt;&gt;"","rxIR proto=4 code="&amp;C25&amp;" (12 bits)",IF(D25&lt;&gt;"","rxRF 1 "&amp;D25,""))</f>
+      <c r="E31" t="s">
+        <v>227</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>rxrf rf.b4.on-&gt;vpstudio.on</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IF(C31&lt;&gt;"","rxIR proto=4 code="&amp;C31&amp;" (12 bits)",IF(D31&lt;&gt;"","rxRF 1 "&amp;D31,""))</f>
         <v>rxRF 1 7fd514</v>
       </c>
-      <c r="H25" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="2"/>
         <v>home/domo/espIR01/event</v>
       </c>
-      <c r="I25" t="str">
+      <c r="I31" t="str">
         <f t="shared" si="3"/>
         <v>rxRF 1 7fd514</v>
       </c>
-      <c r="J25" t="str">
+      <c r="J31" t="str">
         <f t="shared" si="4"/>
-        <v>tvon</v>
-      </c>
-      <c r="K25" t="str">
+        <v>vpstudio.on</v>
+      </c>
+      <c r="K31" t="str">
         <f t="shared" si="5"/>
-        <v>{'comment':'rxrf rf.b4.on-&gt;tvon', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd514', 'command':{'type':'cmdCommand', 'id':'tvon'}},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+        <v>{'comment':'rxrf rf.b4.on-&gt;vpstudio.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd514', 'command':{'type':'cmdCommand', 'id':'vpstudio.on'}},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="1"/>
-        <v>rxrf rf.b4.off-&gt;tvoff</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" ref="G26:G39" si="12">IF(C26&lt;&gt;"","rxIR proto=4 code="&amp;C26&amp;" (12 bits)",IF(D26&lt;&gt;"","rxRF 1 "&amp;D26,""))</f>
+      <c r="E32" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>rxrf rf.b4.off-&gt;vpstudio.off</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" ref="G32:G34" si="12">IF(C32&lt;&gt;"","rxIR proto=4 code="&amp;C32&amp;" (12 bits)",IF(D32&lt;&gt;"","rxRF 1 "&amp;D32,""))</f>
         <v>rxRF 1 7fd511</v>
       </c>
-      <c r="H26" t="str">
+      <c r="H32" t="str">
         <f t="shared" si="2"/>
         <v>home/domo/espIR01/event</v>
       </c>
-      <c r="I26" t="str">
+      <c r="I32" t="str">
         <f t="shared" si="3"/>
         <v>rxRF 1 7fd511</v>
       </c>
-      <c r="J26" t="str">
+      <c r="J32" t="str">
         <f t="shared" si="4"/>
-        <v>tvoff</v>
-      </c>
-      <c r="K26" t="str">
+        <v>vpstudio.off</v>
+      </c>
+      <c r="K32" t="str">
         <f t="shared" si="5"/>
-        <v>{'comment':'rxrf rf.b4.off-&gt;tvoff', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd511', 'command':{'type':'cmdCommand', 'id':'tvoff'}},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+        <v>{'comment':'rxrf rf.b4.off-&gt;vpstudio.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd511', 'command':{'type':'cmdCommand', 'id':'vpstudio.off'}},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E27" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="1"/>
-        <v>rxrf rf.b5.on-&gt;sonOff01.on</v>
-      </c>
-      <c r="G27" t="str">
+      <c r="E33" t="s">
+        <v>229</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>rxrf rf.b5.on-&gt;preamp.mute</v>
+      </c>
+      <c r="G33" t="str">
         <f t="shared" si="12"/>
         <v>rxRF 1 7fd544</v>
       </c>
-      <c r="H27" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="2"/>
         <v>home/domo/espIR01/event</v>
       </c>
-      <c r="I27" t="str">
+      <c r="I33" t="str">
         <f t="shared" si="3"/>
         <v>rxRF 1 7fd544</v>
       </c>
-      <c r="J27" t="str">
+      <c r="J33" t="str">
         <f t="shared" si="4"/>
-        <v>sonOff01.on</v>
-      </c>
-      <c r="K27" t="str">
+        <v>preamp.mute</v>
+      </c>
+      <c r="K33" t="str">
         <f t="shared" si="5"/>
-        <v>{'comment':'rxrf rf.b5.on-&gt;sonOff01.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd544', 'command':{'type':'cmdCommand', 'id':'sonOff01.on'}},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+        <v>{'comment':'rxrf rf.b5.on-&gt;preamp.mute', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd544', 'command':{'type':'cmdCommand', 'id':'preamp.mute'}},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E28" t="s">
-        <v>208</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="1"/>
-        <v>rxrf rf.b5.off-&gt;sonOff01.off</v>
-      </c>
-      <c r="G28" t="str">
+      <c r="F34" t="str">
+        <f t="shared" si="1"/>
+        <v>rxrf rf.b5.off-&gt;</v>
+      </c>
+      <c r="G34" t="str">
         <f t="shared" si="12"/>
         <v>rxRF 1 7fd541</v>
       </c>
-      <c r="H28" t="str">
+      <c r="H34" t="str">
         <f t="shared" si="2"/>
         <v>home/domo/espIR01/event</v>
       </c>
-      <c r="I28" t="str">
+      <c r="I34" t="str">
         <f t="shared" si="3"/>
         <v>rxRF 1 7fd541</v>
       </c>
-      <c r="J28" t="str">
+      <c r="J34" t="str">
         <f t="shared" si="4"/>
-        <v>sonOff01.off</v>
-      </c>
-      <c r="K28" t="str">
+        <v/>
+      </c>
+      <c r="K34" t="str">
         <f t="shared" si="5"/>
-        <v>{'comment':'rxrf rf.b5.off-&gt;sonOff01.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 7fd541', 'command':{'type':'cmdCommand', 'id':'sonOff01.off'}},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" ref="F36:F43" si="13">IF(B36&lt;&gt;"",B36&amp;"-&gt;"&amp;E36,"")</f>
+        <v>rf.d.1.on-&gt;tvon</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" ref="G36:G45" si="14">IF(C36&lt;&gt;"","rxIR proto=4 code="&amp;C36&amp;" (12 bits)",IF(D36&lt;&gt;"","rxRF 1 "&amp;D36,""))</f>
+        <v>rxRF 1 dfc554</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" ref="H36:H45" si="15">IF(OR(C36&lt;&gt;"", D36&lt;&gt;""),"home/domo/espIR01/event","")</f>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" ref="I36:I45" si="16">G36</f>
+        <v>rxRF 1 dfc554</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" ref="J36:J45" si="17">IF(E36&lt;&gt;"",E36,"")</f>
+        <v>tvon</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" ref="K36:K45" si="18">IF(E36&lt;&gt;"","{'comment':'"&amp;F36&amp;"', 'type':'trgMqtt'," &amp;" 'topic':'"&amp;H36&amp;"', 'payload':'"&amp;I36&amp;"', 'command':{'type':'cmdCommand', 'id':'"&amp;J36&amp;"'}},","")</f>
+        <v>{'comment':'rf.d.1.on-&gt;tvon', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfc554', 'command':{'type':'cmdCommand', 'id':'tvon'}},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" ref="F30:F37" si="13">IF(B30&lt;&gt;"",B30&amp;"-&gt;"&amp;E30,"")</f>
-        <v>rf.d.1.on-&gt;tvon</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" ref="G30:G39" si="14">IF(C30&lt;&gt;"","rxIR proto=4 code="&amp;C30&amp;" (12 bits)",IF(D30&lt;&gt;"","rxRF 1 "&amp;D30,""))</f>
-        <v>rxRF 1 dfc554</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" ref="H30:H39" si="15">IF(OR(C30&lt;&gt;"", D30&lt;&gt;""),"home/domo/espIR01/event","")</f>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" ref="I30:I39" si="16">G30</f>
-        <v>rxRF 1 dfc554</v>
-      </c>
-      <c r="J30" t="str">
-        <f t="shared" ref="J30:J39" si="17">IF(E30&lt;&gt;"",E30,"")</f>
-        <v>tvon</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" ref="K30:K39" si="18">IF(E30&lt;&gt;"","{'comment':'"&amp;F30&amp;"', 'type':'trgMqtt'," &amp;" 'topic':'"&amp;H30&amp;"', 'payload':'"&amp;I30&amp;"', 'command':{'type':'cmdCommand', 'id':'"&amp;J30&amp;"'}},","")</f>
-        <v>{'comment':'rf.d.1.on-&gt;tvon', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfc554', 'command':{'type':'cmdCommand', 'id':'tvon'}},</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>214</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E37" t="s">
         <v>48</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F37" t="str">
         <f t="shared" si="13"/>
         <v>rf.d.1.off-&gt;tvoff</v>
       </c>
-      <c r="G31" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="14"/>
         <v>rxRF 1 dfc551</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfc551</v>
-      </c>
-      <c r="J31" t="str">
-        <f t="shared" si="17"/>
-        <v>tvoff</v>
-      </c>
-      <c r="K31" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.1.off-&gt;tvoff', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfc551', 'command':{'type':'cmdCommand', 'id':'tvoff'}},</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>215</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.2.on-&gt;hdmi.1</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd154</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfd154</v>
-      </c>
-      <c r="J32" t="str">
-        <f t="shared" si="17"/>
-        <v>hdmi.1</v>
-      </c>
-      <c r="K32" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.2.on-&gt;hdmi.1', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd154', 'command':{'type':'cmdCommand', 'id':'hdmi.1'}},</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.2.off-&gt;hdmi.2</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd151</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfd151</v>
-      </c>
-      <c r="J33" t="str">
-        <f t="shared" si="17"/>
-        <v>hdmi.2</v>
-      </c>
-      <c r="K33" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.2.off-&gt;hdmi.2', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd151', 'command':{'type':'cmdCommand', 'id':'hdmi.2'}},</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>217</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E34" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.3.on-&gt;hdmi.3</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd454</v>
-      </c>
-      <c r="H34" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I34" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfd454</v>
-      </c>
-      <c r="J34" t="str">
-        <f t="shared" si="17"/>
-        <v>hdmi.3</v>
-      </c>
-      <c r="K34" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.3.on-&gt;hdmi.3', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd454', 'command':{'type':'cmdCommand', 'id':'hdmi.3'}},</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>218</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E35" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.3.off-&gt;hdmi.4</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd451</v>
-      </c>
-      <c r="H35" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I35" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfd451</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="17"/>
-        <v>hdmi.4</v>
-      </c>
-      <c r="K35" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.3.off-&gt;hdmi.4', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd451', 'command':{'type':'cmdCommand', 'id':'hdmi.4'}},</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>219</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E36" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.4.on-&gt;hdmi.5</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd514</v>
-      </c>
-      <c r="H36" t="str">
-        <f t="shared" si="15"/>
-        <v>home/domo/espIR01/event</v>
-      </c>
-      <c r="I36" t="str">
-        <f t="shared" si="16"/>
-        <v>rxRF 1 dfd514</v>
-      </c>
-      <c r="J36" t="str">
-        <f t="shared" si="17"/>
-        <v>hdmi.5</v>
-      </c>
-      <c r="K36" t="str">
-        <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.4.on-&gt;hdmi.5', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd514', 'command':{'type':'cmdCommand', 'id':'hdmi.5'}},</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="13"/>
-        <v>rf.d.4.off-&gt;ampli.mute</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="14"/>
-        <v>rxRF 1 dfd511</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="15"/>
@@ -2285,34 +2123,34 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" si="16"/>
-        <v>rxRF 1 dfd511</v>
+        <v>rxRF 1 dfc551</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="17"/>
-        <v>ampli.mute</v>
+        <v>tvoff</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.4.off-&gt;ampli.mute', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd511', 'command':{'type':'cmdCommand', 'id':'ampli.mute'}},</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{'comment':'rf.d.1.off-&gt;tvoff', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfc551', 'command':{'type':'cmdCommand', 'id':'tvoff'}},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
-        <v>rf.d.5.on-&gt;salon.on</v>
+        <f t="shared" si="13"/>
+        <v>rf.d.2.on-&gt;hdmi.1</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="14"/>
-        <v>rxRF 1 dfd544</v>
+        <v>rxRF 1 dfd154</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="15"/>
@@ -2320,34 +2158,34 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" si="16"/>
-        <v>rxRF 1 dfd544</v>
+        <v>rxRF 1 dfd154</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="17"/>
-        <v>salon.on</v>
+        <v>hdmi.1</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="18"/>
-        <v>{'comment':'rf.d.5.on-&gt;salon.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd544', 'command':{'type':'cmdCommand', 'id':'salon.on'}},</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>{'comment':'rf.d.2.on-&gt;hdmi.1', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd154', 'command':{'type':'cmdCommand', 'id':'hdmi.1'}},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
-        <v>rf.d.5.off-&gt;salon.off</v>
+        <f t="shared" si="13"/>
+        <v>rf.d.2.off-&gt;hdmi.2</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="14"/>
-        <v>rxRF 1 dfd541</v>
+        <v>rxRF 1 dfd151</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="15"/>
@@ -2355,419 +2193,629 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" si="16"/>
-        <v>rxRF 1 dfd541</v>
+        <v>rxRF 1 dfd151</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="17"/>
-        <v>salon.off</v>
+        <v>hdmi.2</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.2.off-&gt;hdmi.2', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd151', 'command':{'type':'cmdCommand', 'id':'hdmi.2'}},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>214</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="13"/>
+        <v>rf.d.3.on-&gt;hdmi.3</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd454</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd454</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="17"/>
+        <v>hdmi.3</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.3.on-&gt;hdmi.3', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd454', 'command':{'type':'cmdCommand', 'id':'hdmi.3'}},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="13"/>
+        <v>rf.d.3.off-&gt;hdmi.4</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd451</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd451</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="17"/>
+        <v>hdmi.4</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.3.off-&gt;hdmi.4', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd451', 'command':{'type':'cmdCommand', 'id':'hdmi.4'}},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="13"/>
+        <v>rf.d.4.on-&gt;hdmi.5</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd514</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd514</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="17"/>
+        <v>hdmi.5</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.4.on-&gt;hdmi.5', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd514', 'command':{'type':'cmdCommand', 'id':'hdmi.5'}},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>217</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="13"/>
+        <v>rf.d.4.off-&gt;ampli.mute</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd511</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd511</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="17"/>
+        <v>ampli.mute</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.4.off-&gt;ampli.mute', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd511', 'command':{'type':'cmdCommand', 'id':'ampli.mute'}},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="1"/>
+        <v>rf.d.5.on-&gt;salon.on</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd544</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd544</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="17"/>
+        <v>salon.on</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="18"/>
+        <v>{'comment':'rf.d.5.on-&gt;salon.on', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd544', 'command':{'type':'cmdCommand', 'id':'salon.on'}},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>219</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="1"/>
+        <v>rf.d.5.off-&gt;salon.off</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="14"/>
+        <v>rxRF 1 dfd541</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="15"/>
+        <v>home/domo/espIR01/event</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="16"/>
+        <v>rxRF 1 dfd541</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="17"/>
+        <v>salon.off</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="18"/>
         <v>{'comment':'rf.d.5.off-&gt;salon.off', 'type':'trgMqtt', 'topic':'home/domo/espIR01/event', 'payload':'rxRF 1 dfd541', 'command':{'type':'cmdCommand', 'id':'salon.off'}},</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>126</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
         <v>136</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>140</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
         <v>148</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
         <v>150</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
         <v>154</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>157</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
         <v>159</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
         <v>160</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>161</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>162</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>163</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
         <v>164</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>165</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
         <v>166</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
         <v>167</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
         <v>168</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
         <v>170</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
         <v>172</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
         <v>174</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D80" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
         <v>176</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>178</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>182</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
         <v>184</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>186</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+      <c r="D86" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>187</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D87" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
         <v>189</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>191</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
         <v>193</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
         <v>195</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D91" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
         <v>197</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
         <v>199</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
         <v>201</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
         <v>203</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
         <v>205</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2785,14 +2833,14 @@
       <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="6.7109375" style="6" customWidth="1"/>
-    <col min="4" max="6" width="9.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="5" customWidth="1"/>
+    <col min="1" max="3" width="6.6640625" style="6" customWidth="1"/>
+    <col min="4" max="6" width="9.5546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>